<commit_message>
Test results for new code
</commit_message>
<xml_diff>
--- a/Important Info/Pokemon Test Results.xlsx
+++ b/Important Info/Pokemon Test Results.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Averages from 10 Tests" sheetId="1" r:id="rId1"/>
-    <sheet name="Newest Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Newest Data" sheetId="2" r:id="rId1"/>
+    <sheet name="Averages from 10 Tests" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="35">
   <si>
     <t>Number of Pokemon: 100</t>
   </si>
@@ -73,14 +73,65 @@
     <t>Max level (50) reached after X iterations:</t>
   </si>
   <si>
-    <t>creating now</t>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Attack</t>
+  </si>
+  <si>
+    <t>Fitness</t>
+  </si>
+  <si>
+    <t>Moves:</t>
+  </si>
+  <si>
+    <t>Average:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quick Attack </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bite </t>
+  </si>
+  <si>
+    <t>Take Down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take Down </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sand Attack </t>
+  </si>
+  <si>
+    <t>Health Probability</t>
+  </si>
+  <si>
+    <t>Attack Probability</t>
+  </si>
+  <si>
+    <t>Defense Probability</t>
+  </si>
+  <si>
+    <t>Total Run Time (seconds)</t>
+  </si>
+  <si>
+    <t>Hybrid</t>
+  </si>
+  <si>
+    <t>Coevolution-1</t>
+  </si>
+  <si>
+    <t>Coevolution-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -130,6 +181,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -139,7 +197,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -167,8 +225,60 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -232,8 +342,80 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -284,8 +466,54 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="13" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="135">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -317,6 +545,42 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -348,6 +612,42 @@
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -356,6 +656,1112 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Highest Level and Final Stats</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hybrid</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$25:$B$28</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Level</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Health</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Attack</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Defense</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Newest Data'!$M$3:$M$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>49.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>138.64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84.52</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>79.52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Coevolution-1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$25:$B$28</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Level</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Health</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Attack</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Defense</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Newest Data'!$M$14:$M$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>119.9399999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>77.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72.92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Coevolution-2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$25:$B$28</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Level</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Health</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Attack</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Defense</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Newest Data'!$M$25:$M$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>21.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90.52999999999988</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.54</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62.54</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2147387432"/>
+        <c:axId val="2147390520"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2147387432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2147390520"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2147390520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2147387432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Stat</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Probabilities</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hybrid</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$29:$B$32</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Health Probability</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Attack Probability</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Defense Probability</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Fitness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Newest Data'!$M$7:$M$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.618601189295364</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.243862587316104</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.137536223388531</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Coevolution-1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$29:$B$32</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Health Probability</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Attack Probability</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Defense Probability</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Fitness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Newest Data'!$M$18:$M$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.916493442643265</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.038346841313692</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0451597160430429</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Coevolution-2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$29:$B$32</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Health Probability</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Attack Probability</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Defense Probability</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Fitness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Newest Data'!$M$29:$M$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.812955091493466</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0951224288250871</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0919224796814462</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2145510568"/>
+        <c:axId val="-2145431768"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2145510568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2145431768"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2145431768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2145510568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Percentage of the Time</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> a </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Move</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> was One of the Pokemon's Three Moves</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hybrid</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Newest Data'!$N$25:$N$28</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Quick Attack </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bite </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Take Down </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sand Attack </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Newest Data'!$O$3:$O$6</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Coevolution-1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Newest Data'!$N$25:$N$28</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Quick Attack </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bite </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Take Down </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sand Attack </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Newest Data'!$O$14:$O$17</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Coevolution-2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Newest Data'!$N$25:$N$28</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Quick Attack </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bite </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Take Down </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sand Attack </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Newest Data'!$O$25:$O$28</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2142665688"/>
+        <c:axId val="-2142662600"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2142665688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2142662600"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2142662600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2142665688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800"/>
+              <a:t>Pokemon</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800"/>
+              <a:t>Fitness and Total Run Time (in seconds)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hybrid</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fitness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Newest Data'!$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.017003084257831</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Coevolution-1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fitness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Newest Data'!$M$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5.496909110651162</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Coevolution-2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fitness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Newest Data'!$M$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.742407499850204</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Run Time (seconds)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Newest Data'!$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fitness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Newest Data'!$M$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.5969</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2145093384"/>
+        <c:axId val="2145196056"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2145093384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2145196056"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2145196056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2145093384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -598,11 +2004,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2104806424"/>
-        <c:axId val="2136506648"/>
+        <c:axId val="2141230152"/>
+        <c:axId val="2141227160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2104806424"/>
+        <c:axId val="2141230152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -611,7 +2017,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2136506648"/>
+        <c:crossAx val="2141227160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -619,7 +2025,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2136506648"/>
+        <c:axId val="2141227160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -630,7 +2036,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2104806424"/>
+        <c:crossAx val="2141230152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -652,7 +2058,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -821,11 +2227,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2104728216"/>
-        <c:axId val="2104725224"/>
+        <c:axId val="2135570376"/>
+        <c:axId val="2135631560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2104728216"/>
+        <c:axId val="2135570376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -834,7 +2240,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2104725224"/>
+        <c:crossAx val="2135631560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -842,7 +2248,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2104725224"/>
+        <c:axId val="2135631560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -853,7 +2259,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2104728216"/>
+        <c:crossAx val="2135570376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -876,6 +2282,131 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1262,9 +2793,1269 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:O36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC16" sqref="AC16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.1640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.1640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.1640625" style="36" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" ht="16" thickBot="1">
+      <c r="B2" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="M2" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="34"/>
+    </row>
+    <row r="3" spans="2:15">
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="22">
+        <v>50</v>
+      </c>
+      <c r="D3" s="22">
+        <v>50</v>
+      </c>
+      <c r="E3" s="22">
+        <v>50</v>
+      </c>
+      <c r="F3" s="22">
+        <v>50</v>
+      </c>
+      <c r="G3" s="22">
+        <v>50</v>
+      </c>
+      <c r="H3" s="22">
+        <v>50</v>
+      </c>
+      <c r="I3" s="22">
+        <v>50</v>
+      </c>
+      <c r="J3" s="22">
+        <v>49</v>
+      </c>
+      <c r="K3" s="22">
+        <v>50</v>
+      </c>
+      <c r="L3" s="22">
+        <v>50</v>
+      </c>
+      <c r="M3" s="28">
+        <f>AVERAGE(C3:L3)</f>
+        <v>49.9</v>
+      </c>
+      <c r="N3" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15">
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="22">
+        <v>138.30000000000001</v>
+      </c>
+      <c r="D4" s="22">
+        <v>138.30000000000001</v>
+      </c>
+      <c r="E4" s="22">
+        <v>138.30000000000001</v>
+      </c>
+      <c r="F4" s="22">
+        <v>140</v>
+      </c>
+      <c r="G4" s="22">
+        <v>138.30000000000001</v>
+      </c>
+      <c r="H4" s="22">
+        <v>140</v>
+      </c>
+      <c r="I4" s="22">
+        <v>138.30000000000001</v>
+      </c>
+      <c r="J4" s="22">
+        <v>136.6</v>
+      </c>
+      <c r="K4" s="22">
+        <v>138.30000000000001</v>
+      </c>
+      <c r="L4" s="22">
+        <v>140</v>
+      </c>
+      <c r="M4" s="29">
+        <f t="shared" ref="M4:M10" si="0">AVERAGE(C4:L4)</f>
+        <v>138.63999999999999</v>
+      </c>
+      <c r="N4" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15">
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="22">
+        <v>84.4</v>
+      </c>
+      <c r="D5" s="22">
+        <v>84.4</v>
+      </c>
+      <c r="E5" s="22">
+        <v>84.4</v>
+      </c>
+      <c r="F5" s="22">
+        <v>85</v>
+      </c>
+      <c r="G5" s="22">
+        <v>84.4</v>
+      </c>
+      <c r="H5" s="22">
+        <v>85</v>
+      </c>
+      <c r="I5" s="22">
+        <v>84.4</v>
+      </c>
+      <c r="J5" s="22">
+        <v>83.8</v>
+      </c>
+      <c r="K5" s="22">
+        <v>84.4</v>
+      </c>
+      <c r="L5" s="22">
+        <v>85</v>
+      </c>
+      <c r="M5" s="29">
+        <f t="shared" si="0"/>
+        <v>84.52</v>
+      </c>
+      <c r="N5" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15">
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="22">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="D6" s="22">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="E6" s="22">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="F6" s="22">
+        <v>80</v>
+      </c>
+      <c r="G6" s="22">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="H6" s="22">
+        <v>80</v>
+      </c>
+      <c r="I6" s="22">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="J6" s="22">
+        <v>78.8</v>
+      </c>
+      <c r="K6" s="22">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="L6" s="22">
+        <v>80</v>
+      </c>
+      <c r="M6" s="29">
+        <f t="shared" si="0"/>
+        <v>79.52</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15">
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="22">
+        <v>0.47582094366191202</v>
+      </c>
+      <c r="D7" s="22">
+        <v>0.33982653558054698</v>
+      </c>
+      <c r="E7" s="22">
+        <v>0.51700018237613399</v>
+      </c>
+      <c r="F7" s="22">
+        <v>0.53791978359722903</v>
+      </c>
+      <c r="G7" s="22">
+        <v>0.93357014877470701</v>
+      </c>
+      <c r="H7" s="22">
+        <v>1</v>
+      </c>
+      <c r="I7" s="22">
+        <v>0.488456813176327</v>
+      </c>
+      <c r="J7" s="22">
+        <v>0.59419671137018104</v>
+      </c>
+      <c r="K7" s="22">
+        <v>0.68522133094379001</v>
+      </c>
+      <c r="L7" s="22">
+        <v>0.61399944347281499</v>
+      </c>
+      <c r="M7" s="37">
+        <f>AVERAGE(C7:L7)</f>
+        <v>0.61860118929536412</v>
+      </c>
+      <c r="N7" s="22"/>
+      <c r="O7" s="34"/>
+    </row>
+    <row r="8" spans="2:15">
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="22">
+        <v>0.52417905633808703</v>
+      </c>
+      <c r="D8" s="22">
+        <v>0.31869928848657098</v>
+      </c>
+      <c r="E8" s="22">
+        <v>8.0354077812206701E-2</v>
+      </c>
+      <c r="F8" s="22">
+        <v>0.46208021640277003</v>
+      </c>
+      <c r="G8" s="22">
+        <v>6.6429851225292699E-2</v>
+      </c>
+      <c r="H8" s="22">
+        <v>0</v>
+      </c>
+      <c r="I8" s="22">
+        <v>4.6400536422088502E-2</v>
+      </c>
+      <c r="J8" s="22">
+        <v>0.29758604489859303</v>
+      </c>
+      <c r="K8" s="22">
+        <v>0.31477866905620999</v>
+      </c>
+      <c r="L8" s="22">
+        <v>0.328118132519225</v>
+      </c>
+      <c r="M8" s="37">
+        <f>AVERAGE(C8:L8)</f>
+        <v>0.24386258731610438</v>
+      </c>
+      <c r="N8" s="22"/>
+      <c r="O8" s="34"/>
+    </row>
+    <row r="9" spans="2:15">
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="22">
+        <v>0</v>
+      </c>
+      <c r="D9" s="22">
+        <v>0.34147417593288099</v>
+      </c>
+      <c r="E9" s="22">
+        <v>0.40264573981165902</v>
+      </c>
+      <c r="F9" s="22">
+        <v>0</v>
+      </c>
+      <c r="G9" s="22">
+        <v>0</v>
+      </c>
+      <c r="H9" s="22">
+        <v>0</v>
+      </c>
+      <c r="I9" s="22">
+        <v>0.46514265040158298</v>
+      </c>
+      <c r="J9" s="22">
+        <v>0.108217243731224</v>
+      </c>
+      <c r="K9" s="22">
+        <v>0</v>
+      </c>
+      <c r="L9" s="22">
+        <v>5.7882424007959003E-2</v>
+      </c>
+      <c r="M9" s="37">
+        <f>AVERAGE(C9:L9)</f>
+        <v>0.13753622338853061</v>
+      </c>
+      <c r="N9" s="22"/>
+      <c r="O9" s="34"/>
+    </row>
+    <row r="10" spans="2:15" ht="16" thickBot="1">
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="22">
+        <v>6.7370111020863002</v>
+      </c>
+      <c r="D10" s="22">
+        <v>6.7397598225403996</v>
+      </c>
+      <c r="E10" s="22">
+        <v>7.2964206267295797</v>
+      </c>
+      <c r="F10" s="22">
+        <v>7.6241352364215897</v>
+      </c>
+      <c r="G10" s="22">
+        <v>7.3669565173460798</v>
+      </c>
+      <c r="H10" s="22">
+        <v>7.9400928855919597</v>
+      </c>
+      <c r="I10" s="22">
+        <v>4.3939520938444501</v>
+      </c>
+      <c r="J10" s="22">
+        <v>7.6241849228045</v>
+      </c>
+      <c r="K10" s="22">
+        <v>6.8764088671819898</v>
+      </c>
+      <c r="L10" s="22">
+        <v>7.5711087680314701</v>
+      </c>
+      <c r="M10" s="30">
+        <f t="shared" si="0"/>
+        <v>7.0170030842578317</v>
+      </c>
+      <c r="N10" s="22"/>
+      <c r="O10" s="34"/>
+    </row>
+    <row r="11" spans="2:15">
+      <c r="B11" s="1"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="34"/>
+    </row>
+    <row r="12" spans="2:15">
+      <c r="B12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="34"/>
+    </row>
+    <row r="13" spans="2:15" ht="16" thickBot="1">
+      <c r="B13" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="M13" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="N13" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="34"/>
+    </row>
+    <row r="14" spans="2:15">
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="22">
+        <v>20</v>
+      </c>
+      <c r="D14" s="22">
+        <v>50</v>
+      </c>
+      <c r="E14" s="22">
+        <v>19</v>
+      </c>
+      <c r="F14" s="22">
+        <v>32</v>
+      </c>
+      <c r="G14" s="22">
+        <v>50</v>
+      </c>
+      <c r="H14" s="22">
+        <v>50</v>
+      </c>
+      <c r="I14" s="22">
+        <v>50</v>
+      </c>
+      <c r="J14" s="22">
+        <v>43</v>
+      </c>
+      <c r="K14" s="22">
+        <v>50</v>
+      </c>
+      <c r="L14" s="22">
+        <v>26</v>
+      </c>
+      <c r="M14" s="28">
+        <f>AVERAGE(C14:L14)</f>
+        <v>39</v>
+      </c>
+      <c r="N14" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="O14" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15">
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="22">
+        <v>87.3</v>
+      </c>
+      <c r="D15" s="22">
+        <v>138.30000000000001</v>
+      </c>
+      <c r="E15" s="22">
+        <v>85.6</v>
+      </c>
+      <c r="F15" s="22">
+        <v>107.69999999999899</v>
+      </c>
+      <c r="G15" s="22">
+        <v>140</v>
+      </c>
+      <c r="H15" s="22">
+        <v>138.30000000000001</v>
+      </c>
+      <c r="I15" s="22">
+        <v>138.30000000000001</v>
+      </c>
+      <c r="J15" s="22">
+        <v>126.399999999999</v>
+      </c>
+      <c r="K15" s="22">
+        <v>140</v>
+      </c>
+      <c r="L15" s="22">
+        <v>97.5</v>
+      </c>
+      <c r="M15" s="29">
+        <f t="shared" ref="M15:M21" si="1">AVERAGE(C15:L15)</f>
+        <v>119.9399999999998</v>
+      </c>
+      <c r="N15" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="O15" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15">
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="22">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="D16" s="22">
+        <v>84.4</v>
+      </c>
+      <c r="E16" s="22">
+        <v>65.8</v>
+      </c>
+      <c r="F16" s="22">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="G16" s="22">
+        <v>85</v>
+      </c>
+      <c r="H16" s="22">
+        <v>84.4</v>
+      </c>
+      <c r="I16" s="22">
+        <v>84.4</v>
+      </c>
+      <c r="J16" s="22">
+        <v>80.2</v>
+      </c>
+      <c r="K16" s="22">
+        <v>85</v>
+      </c>
+      <c r="L16" s="22">
+        <v>70</v>
+      </c>
+      <c r="M16" s="29">
+        <f t="shared" si="1"/>
+        <v>77.92</v>
+      </c>
+      <c r="N16" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="O16" s="35">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15">
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="22">
+        <v>61.4</v>
+      </c>
+      <c r="D17" s="22">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="E17" s="22">
+        <v>60.8</v>
+      </c>
+      <c r="F17" s="22">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="G17" s="22">
+        <v>80</v>
+      </c>
+      <c r="H17" s="22">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="I17" s="22">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="J17" s="22">
+        <v>75.2</v>
+      </c>
+      <c r="K17" s="22">
+        <v>80</v>
+      </c>
+      <c r="L17" s="22">
+        <v>65</v>
+      </c>
+      <c r="M17" s="29">
+        <f t="shared" si="1"/>
+        <v>72.92</v>
+      </c>
+      <c r="N17" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="O17" s="35">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15">
+      <c r="B18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="22">
+        <v>0.76666048026842304</v>
+      </c>
+      <c r="D18" s="22">
+        <v>1</v>
+      </c>
+      <c r="E18" s="22">
+        <v>0.87751382803669897</v>
+      </c>
+      <c r="F18" s="22">
+        <v>0.87775331713493498</v>
+      </c>
+      <c r="G18" s="22">
+        <v>0.86313720679535999</v>
+      </c>
+      <c r="H18" s="22">
+        <v>1</v>
+      </c>
+      <c r="I18" s="22">
+        <v>1</v>
+      </c>
+      <c r="J18" s="22">
+        <v>0.99509092546954403</v>
+      </c>
+      <c r="K18" s="22">
+        <v>0.99324414487796797</v>
+      </c>
+      <c r="L18" s="22">
+        <v>0.79153452384971701</v>
+      </c>
+      <c r="M18" s="37">
+        <f>AVERAGE(C18:L18)</f>
+        <v>0.9164934426432646</v>
+      </c>
+      <c r="N18" s="22"/>
+      <c r="O18" s="35"/>
+    </row>
+    <row r="19" spans="2:15">
+      <c r="B19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="22">
+        <v>0.17009386245618299</v>
+      </c>
+      <c r="D19" s="22">
+        <v>0</v>
+      </c>
+      <c r="E19" s="22">
+        <v>0</v>
+      </c>
+      <c r="F19" s="22">
+        <v>0</v>
+      </c>
+      <c r="G19" s="22">
+        <v>0</v>
+      </c>
+      <c r="H19" s="22">
+        <v>0</v>
+      </c>
+      <c r="I19" s="22">
+        <v>0</v>
+      </c>
+      <c r="J19" s="22">
+        <v>4.9090745304552902E-3</v>
+      </c>
+      <c r="K19" s="22">
+        <v>0</v>
+      </c>
+      <c r="L19" s="22">
+        <v>0.20846547615028199</v>
+      </c>
+      <c r="M19" s="37">
+        <f>AVERAGE(C19:L19)</f>
+        <v>3.8346841313692023E-2</v>
+      </c>
+      <c r="N19" s="22"/>
+      <c r="O19" s="34"/>
+    </row>
+    <row r="20" spans="2:15">
+      <c r="B20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="22">
+        <v>6.3245657275393899E-2</v>
+      </c>
+      <c r="D20" s="22">
+        <v>0</v>
+      </c>
+      <c r="E20" s="22">
+        <v>0.122486171963301</v>
+      </c>
+      <c r="F20" s="22">
+        <v>0.122246682865064</v>
+      </c>
+      <c r="G20" s="22">
+        <v>0.13686279320463901</v>
+      </c>
+      <c r="H20" s="22">
+        <v>0</v>
+      </c>
+      <c r="I20" s="22">
+        <v>0</v>
+      </c>
+      <c r="J20" s="22">
+        <v>0</v>
+      </c>
+      <c r="K20" s="22">
+        <v>6.7558551220313597E-3</v>
+      </c>
+      <c r="L20" s="22">
+        <v>0</v>
+      </c>
+      <c r="M20" s="37">
+        <f>AVERAGE(C20:L20)</f>
+        <v>4.5159716043042933E-2</v>
+      </c>
+      <c r="N20" s="22"/>
+      <c r="O20" s="34"/>
+    </row>
+    <row r="21" spans="2:15" ht="16" thickBot="1">
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="22">
+        <v>4.4340729841922997</v>
+      </c>
+      <c r="D21" s="22">
+        <v>7.0036450674349497</v>
+      </c>
+      <c r="E21" s="22">
+        <v>4.2477473070689404</v>
+      </c>
+      <c r="F21" s="22">
+        <v>5.5132236754508996</v>
+      </c>
+      <c r="G21" s="22">
+        <v>5.6191013193504302</v>
+      </c>
+      <c r="H21" s="22">
+        <v>5.4337836382194098</v>
+      </c>
+      <c r="I21" s="22">
+        <v>8.1431614179499192</v>
+      </c>
+      <c r="J21" s="22">
+        <v>3.5014392526410099</v>
+      </c>
+      <c r="K21" s="22">
+        <v>5.1893220488092204</v>
+      </c>
+      <c r="L21" s="22">
+        <v>5.8835943953945504</v>
+      </c>
+      <c r="M21" s="30">
+        <f t="shared" si="1"/>
+        <v>5.4969091106511625</v>
+      </c>
+      <c r="N21" s="22"/>
+      <c r="O21" s="34"/>
+    </row>
+    <row r="22" spans="2:15">
+      <c r="B22" s="1"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="34"/>
+    </row>
+    <row r="23" spans="2:15">
+      <c r="B23" s="1"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="34"/>
+    </row>
+    <row r="24" spans="2:15" ht="16" thickBot="1">
+      <c r="B24" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="M24" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="N24" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="O24" s="34"/>
+    </row>
+    <row r="25" spans="2:15">
+      <c r="B25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="22">
+        <v>22</v>
+      </c>
+      <c r="D25" s="22">
+        <v>8</v>
+      </c>
+      <c r="E25" s="22">
+        <v>50</v>
+      </c>
+      <c r="F25" s="22">
+        <v>12</v>
+      </c>
+      <c r="G25" s="22">
+        <v>32</v>
+      </c>
+      <c r="H25" s="22">
+        <v>14</v>
+      </c>
+      <c r="I25" s="22">
+        <v>14</v>
+      </c>
+      <c r="J25" s="22">
+        <v>29</v>
+      </c>
+      <c r="K25" s="22">
+        <v>27</v>
+      </c>
+      <c r="L25" s="22">
+        <v>10</v>
+      </c>
+      <c r="M25" s="28">
+        <f>AVERAGE(C25:L25)</f>
+        <v>21.8</v>
+      </c>
+      <c r="N25" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="O25" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15">
+      <c r="B26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="22">
+        <v>90.699999999999903</v>
+      </c>
+      <c r="D26" s="22">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="E26" s="22">
+        <v>140</v>
+      </c>
+      <c r="F26" s="22">
+        <v>73.7</v>
+      </c>
+      <c r="G26" s="22">
+        <v>107.69999999999899</v>
+      </c>
+      <c r="H26" s="22">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="I26" s="22">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="J26" s="22">
+        <v>102.6</v>
+      </c>
+      <c r="K26" s="22">
+        <v>99.199999999999903</v>
+      </c>
+      <c r="L26" s="22">
+        <v>70.3</v>
+      </c>
+      <c r="M26" s="29">
+        <f t="shared" ref="M26:M32" si="2">AVERAGE(C26:L26)</f>
+        <v>90.529999999999887</v>
+      </c>
+      <c r="N26" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="O26" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15">
+      <c r="B27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="22">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="D27" s="22">
+        <v>59.2</v>
+      </c>
+      <c r="E27" s="22">
+        <v>85</v>
+      </c>
+      <c r="F27" s="22">
+        <v>61.6</v>
+      </c>
+      <c r="G27" s="22">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="H27" s="22">
+        <v>62.8</v>
+      </c>
+      <c r="I27" s="22">
+        <v>62.8</v>
+      </c>
+      <c r="J27" s="22">
+        <v>71.8</v>
+      </c>
+      <c r="K27" s="22">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="L27" s="22">
+        <v>60.4</v>
+      </c>
+      <c r="M27" s="29">
+        <f t="shared" si="2"/>
+        <v>67.539999999999992</v>
+      </c>
+      <c r="N27" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="O27" s="35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15">
+      <c r="B28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="22">
+        <v>62.6</v>
+      </c>
+      <c r="D28" s="22">
+        <v>54.2</v>
+      </c>
+      <c r="E28" s="22">
+        <v>80</v>
+      </c>
+      <c r="F28" s="22">
+        <v>56.6</v>
+      </c>
+      <c r="G28" s="22">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="H28" s="22">
+        <v>57.8</v>
+      </c>
+      <c r="I28" s="22">
+        <v>57.8</v>
+      </c>
+      <c r="J28" s="22">
+        <v>66.8</v>
+      </c>
+      <c r="K28" s="22">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="L28" s="22">
+        <v>55.4</v>
+      </c>
+      <c r="M28" s="29">
+        <f t="shared" si="2"/>
+        <v>62.54</v>
+      </c>
+      <c r="N28" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="O28" s="35">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15">
+      <c r="B29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="22">
+        <v>0.86645408063739204</v>
+      </c>
+      <c r="D29" s="22">
+        <v>0.88164776170570303</v>
+      </c>
+      <c r="E29" s="22">
+        <v>1</v>
+      </c>
+      <c r="F29" s="22">
+        <v>1</v>
+      </c>
+      <c r="G29" s="22">
+        <v>1</v>
+      </c>
+      <c r="H29" s="22">
+        <v>0.79396905045782895</v>
+      </c>
+      <c r="I29" s="22">
+        <v>0.53294175376377995</v>
+      </c>
+      <c r="J29" s="22">
+        <v>0.63122469257011804</v>
+      </c>
+      <c r="K29" s="22">
+        <v>0.72389696856255303</v>
+      </c>
+      <c r="L29" s="22">
+        <v>0.69941660723728205</v>
+      </c>
+      <c r="M29" s="37">
+        <f>AVERAGE(C29:L29)</f>
+        <v>0.81295509149346556</v>
+      </c>
+      <c r="N29" s="22"/>
+      <c r="O29" s="34"/>
+    </row>
+    <row r="30" spans="2:15">
+      <c r="B30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="22">
+        <v>3.06809526381727E-2</v>
+      </c>
+      <c r="D30" s="22">
+        <v>0.118352238294296</v>
+      </c>
+      <c r="E30" s="22">
+        <v>0</v>
+      </c>
+      <c r="F30" s="22">
+        <v>0</v>
+      </c>
+      <c r="G30" s="22">
+        <v>0</v>
+      </c>
+      <c r="H30" s="22">
+        <v>0.13674227602931099</v>
+      </c>
+      <c r="I30" s="22">
+        <v>0.282569650267888</v>
+      </c>
+      <c r="J30" s="22">
+        <v>0.164405447167601</v>
+      </c>
+      <c r="K30" s="22">
+        <v>0.218473723853603</v>
+      </c>
+      <c r="L30" s="22">
+        <v>0</v>
+      </c>
+      <c r="M30" s="37">
+        <f>AVERAGE(C30:L30)</f>
+        <v>9.512242882508716E-2</v>
+      </c>
+      <c r="N30" s="22"/>
+      <c r="O30" s="34"/>
+    </row>
+    <row r="31" spans="2:15">
+      <c r="B31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="22">
+        <v>0.102864966724434</v>
+      </c>
+      <c r="D31" s="22">
+        <v>0</v>
+      </c>
+      <c r="E31" s="22">
+        <v>0</v>
+      </c>
+      <c r="F31" s="22">
+        <v>0</v>
+      </c>
+      <c r="G31" s="22">
+        <v>0</v>
+      </c>
+      <c r="H31" s="22">
+        <v>6.9288673512858501E-2</v>
+      </c>
+      <c r="I31" s="22">
+        <v>0.18448859596833</v>
+      </c>
+      <c r="J31" s="22">
+        <v>0.20436986026227999</v>
+      </c>
+      <c r="K31" s="22">
+        <v>5.7629307583843201E-2</v>
+      </c>
+      <c r="L31" s="22">
+        <v>0.30058339276271701</v>
+      </c>
+      <c r="M31" s="37">
+        <f>AVERAGE(C31:L31)</f>
+        <v>9.1922479681446262E-2</v>
+      </c>
+      <c r="N31" s="22"/>
+      <c r="O31" s="34"/>
+    </row>
+    <row r="32" spans="2:15" ht="16" thickBot="1">
+      <c r="B32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="22">
+        <v>6.6940061367472499</v>
+      </c>
+      <c r="D32" s="22">
+        <v>8.9390003858857803</v>
+      </c>
+      <c r="E32" s="22">
+        <v>7.0888087122129999</v>
+      </c>
+      <c r="F32" s="22">
+        <v>3.0527837311146602</v>
+      </c>
+      <c r="G32" s="22">
+        <v>3.95344111801381</v>
+      </c>
+      <c r="H32" s="22">
+        <v>3.0494100729390401</v>
+      </c>
+      <c r="I32" s="22">
+        <v>1.66259705851814</v>
+      </c>
+      <c r="J32" s="22">
+        <v>6.74505545124007</v>
+      </c>
+      <c r="K32" s="22">
+        <v>3.49168719462681</v>
+      </c>
+      <c r="L32" s="22">
+        <v>2.7472851372034701</v>
+      </c>
+      <c r="M32" s="30">
+        <f t="shared" si="2"/>
+        <v>4.7424074998502039</v>
+      </c>
+      <c r="N32" s="22"/>
+      <c r="O32" s="34"/>
+    </row>
+    <row r="33" spans="2:15">
+      <c r="B33" s="1"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="25"/>
+      <c r="L33" s="25"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="34"/>
+    </row>
+    <row r="34" spans="2:15" ht="16" thickBot="1">
+      <c r="B34" s="1"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="M34" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="N34" s="27"/>
+      <c r="O34" s="34"/>
+    </row>
+    <row r="35" spans="2:15" ht="16" thickBot="1">
+      <c r="B35" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="22">
+        <v>2.8130000000000002</v>
+      </c>
+      <c r="D35" s="22">
+        <v>0.59</v>
+      </c>
+      <c r="E35" s="22">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="F35" s="22">
+        <v>3.05</v>
+      </c>
+      <c r="G35" s="22">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="H35" s="22">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="I35" s="22">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="J35" s="22">
+        <v>3.5979999999999999</v>
+      </c>
+      <c r="K35" s="22">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="L35" s="22">
+        <v>2.169</v>
+      </c>
+      <c r="M35" s="33">
+        <f>AVERAGE(C35:L35)</f>
+        <v>1.5969000000000002</v>
+      </c>
+      <c r="N35" s="1"/>
+      <c r="O35" s="34"/>
+    </row>
+    <row r="36" spans="2:15">
+      <c r="B36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="34"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:XFD40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B32" sqref="B32:B39"/>
     </sheetView>
   </sheetViews>
@@ -18886,29 +21677,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="3" spans="2:2">
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>